<commit_message>
Phase One Progress (1)
- Implemented more of the ISA (conditional branch, subroutines, etc...)
- Ability to create comments in mia assembly files
- Tweaked how the call stack works
- Bug fixes
</commit_message>
<xml_diff>
--- a/docs/ISA.xlsx
+++ b/docs/ISA.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jeremy/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jeremy/Desktop/Project-Maya/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2740" yWindow="1380" windowWidth="22880" windowHeight="15260" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14360" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="262">
   <si>
     <t>Instruction</t>
   </si>
@@ -239,15 +239,6 @@
     <t>cmp</t>
   </si>
   <si>
-    <t>castl</t>
-  </si>
-  <si>
-    <t>castw</t>
-  </si>
-  <si>
-    <t>castb</t>
-  </si>
-  <si>
     <t>cmpfs</t>
   </si>
   <si>
@@ -500,15 +491,6 @@
     <t>testz</t>
   </si>
   <si>
-    <t>lfmq</t>
-  </si>
-  <si>
-    <t>lfmw</t>
-  </si>
-  <si>
-    <t>lfmb</t>
-  </si>
-  <si>
     <t>0x80</t>
   </si>
   <si>
@@ -749,9 +731,6 @@
     <t>2b imm</t>
   </si>
   <si>
-    <t>1 b imm</t>
-  </si>
-  <si>
     <t>4b imm</t>
   </si>
   <si>
@@ -764,7 +743,76 @@
     <t>imm first binary</t>
   </si>
   <si>
-    <t>lfml</t>
+    <t>testl</t>
+  </si>
+  <si>
+    <t>testw</t>
+  </si>
+  <si>
+    <t>testb</t>
+  </si>
+  <si>
+    <t>lml</t>
+  </si>
+  <si>
+    <t>lmq</t>
+  </si>
+  <si>
+    <t>lmw</t>
+  </si>
+  <si>
+    <t>lmb</t>
+  </si>
+  <si>
+    <t>0x3b</t>
+  </si>
+  <si>
+    <t>0x3a</t>
+  </si>
+  <si>
+    <t>0x3c</t>
+  </si>
+  <si>
+    <t>0x3d</t>
+  </si>
+  <si>
+    <t>addb</t>
+  </si>
+  <si>
+    <t>addw</t>
+  </si>
+  <si>
+    <t>addq</t>
+  </si>
+  <si>
+    <t>addl</t>
+  </si>
+  <si>
+    <t>subq</t>
+  </si>
+  <si>
+    <t>subl</t>
+  </si>
+  <si>
+    <t>subw</t>
+  </si>
+  <si>
+    <t>subb</t>
+  </si>
+  <si>
+    <t>0x3e</t>
+  </si>
+  <si>
+    <t>0x3f</t>
+  </si>
+  <si>
+    <t>0x46</t>
+  </si>
+  <si>
+    <t>0x47</t>
+  </si>
+  <si>
+    <t>1b imm</t>
   </si>
 </sst>
 </file>
@@ -793,7 +841,7 @@
       <name val="Monaco"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -872,6 +920,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -885,7 +939,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -893,16 +947,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -921,12 +969,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -939,25 +981,40 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1237,16 +1294,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X91"/>
+  <dimension ref="A1:X99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="H78" sqref="H78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="10.83203125" style="15"/>
+    <col min="2" max="2" width="10.83203125" style="11"/>
     <col min="3" max="6" width="10.83203125" style="2"/>
     <col min="7" max="7" width="17.33203125" style="2" customWidth="1"/>
     <col min="8" max="8" width="23.5" style="2" customWidth="1"/>
@@ -1262,7 +1319,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -1282,28 +1339,28 @@
       <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
+      <c r="X1" s="17"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>160</v>
+      <c r="A2" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>154</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>9</v>
@@ -1318,10 +1375,10 @@
         <v>20</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>219</v>
+        <v>237</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>213</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>15</v>
@@ -1332,18 +1389,18 @@
       <c r="L2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3" t="s">
+      <c r="N2" s="17"/>
+      <c r="O2" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3" t="s">
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="R2" s="3"/>
+      <c r="R2" s="17"/>
       <c r="S2" s="1" t="s">
         <v>54</v>
       </c>
@@ -1364,11 +1421,11 @@
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A3" s="18" t="s">
-        <v>245</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>161</v>
+      <c r="A3" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>9</v>
@@ -1383,41 +1440,41 @@
         <v>20</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="H3" s="13"/>
-      <c r="J3" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="H3" s="20"/>
+      <c r="J3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="9">
+      <c r="K3" s="7">
         <v>10</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="10"/>
-      <c r="N3" s="5" t="s">
+      <c r="M3" s="8"/>
+      <c r="N3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="O3" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
+      <c r="O3" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
+      <c r="S3" s="18"/>
+      <c r="T3" s="18"/>
+      <c r="U3" s="18"/>
+      <c r="V3" s="18"/>
+      <c r="W3" s="18"/>
+      <c r="X3" s="18"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A4" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>163</v>
+      <c r="A4" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>157</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>9</v>
@@ -1432,38 +1489,38 @@
         <v>20</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="H4" s="13"/>
+        <v>237</v>
+      </c>
+      <c r="H4" s="20"/>
       <c r="J4" s="2" t="s">
         <v>43</v>
       </c>
       <c r="K4" s="2">
         <v>9</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="M4" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="6"/>
-      <c r="W4" s="6"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="18"/>
+      <c r="S4" s="18"/>
+      <c r="T4" s="18"/>
+      <c r="U4" s="18"/>
+      <c r="V4" s="18"/>
+      <c r="W4" s="18"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>159</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>165</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>9</v>
@@ -1478,26 +1535,26 @@
         <v>20</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="H5" s="13"/>
-      <c r="J5" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="H5" s="20"/>
+      <c r="J5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="9">
+      <c r="K5" s="7">
         <v>3</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="L5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M5" s="10"/>
-      <c r="N5" s="5" t="s">
+      <c r="M5" s="8"/>
+      <c r="N5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="O5" s="7" t="s">
+      <c r="O5" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="P5" s="8" t="s">
+      <c r="P5" s="6" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1505,8 +1562,8 @@
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="15" t="s">
-        <v>166</v>
+      <c r="B6" s="11" t="s">
+        <v>160</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>9</v>
@@ -1529,13 +1586,13 @@
       <c r="K6" s="2">
         <v>2</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="L6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M6" s="7" t="s">
+      <c r="M6" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="N6" s="5" t="s">
+      <c r="N6" s="4" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1543,8 +1600,8 @@
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="15" t="s">
-        <v>167</v>
+      <c r="B7" s="11" t="s">
+        <v>161</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>9</v>
@@ -1567,27 +1624,27 @@
       <c r="K7" s="2">
         <v>2</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="L7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M7" s="10"/>
-      <c r="N7" s="5" t="s">
+      <c r="M7" s="8"/>
+      <c r="N7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="12"/>
-      <c r="S7" s="12"/>
-      <c r="T7" s="12"/>
-      <c r="U7" s="12"/>
-      <c r="V7" s="12"/>
-      <c r="W7" s="12"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="15" t="s">
-        <v>168</v>
+      <c r="B8" s="11" t="s">
+        <v>162</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>9</v>
@@ -1610,7 +1667,7 @@
       <c r="K8" s="2">
         <v>1</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="L8" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1618,8 +1675,8 @@
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>169</v>
+      <c r="B9" s="11" t="s">
+        <v>163</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>9</v>
@@ -1636,352 +1693,352 @@
       <c r="G9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="J9" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="K9" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="L9" s="4" t="s">
+      <c r="K9" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="L9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M9" s="10"/>
-      <c r="N9" s="22" t="s">
+      <c r="M9" s="8"/>
+      <c r="N9" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="O9" s="24" t="s">
-        <v>240</v>
-      </c>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="R9" s="6"/>
-      <c r="S9" s="23" t="s">
-        <v>241</v>
-      </c>
-      <c r="T9" s="23"/>
+      <c r="O9" s="23" t="s">
+        <v>261</v>
+      </c>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="18" t="s">
+        <v>233</v>
+      </c>
+      <c r="R9" s="18"/>
+      <c r="S9" s="24" t="s">
+        <v>234</v>
+      </c>
+      <c r="T9" s="24"/>
       <c r="U9" s="25" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="V9" s="25"/>
       <c r="W9" s="25"/>
       <c r="X9" s="25"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="20"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="20"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="20"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A15" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="19"/>
+      <c r="J15" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="K15" s="17"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="T15" s="17"/>
+      <c r="U15" s="17"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>243</v>
-      </c>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="11"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="11"/>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A11" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="15" t="s">
+      <c r="C16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="19"/>
+      <c r="J16" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="K16" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="T16" s="21" t="s">
+        <v>215</v>
+      </c>
+      <c r="U16" s="19" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A17" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="13"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="11"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="11"/>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A12" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" s="13"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="11"/>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="11"/>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A13" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="13"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="11"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="11"/>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A14" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>243</v>
-      </c>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="11"/>
-      <c r="O14" s="11"/>
-      <c r="P14" s="11"/>
-      <c r="Q14" s="11"/>
-      <c r="R14" s="11"/>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A15" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="15" t="s">
+      <c r="C17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="19"/>
+      <c r="J17" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H15" s="14"/>
-      <c r="J15" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="K15" s="3"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="11"/>
-      <c r="S15" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="T15" s="3"/>
-      <c r="U15" s="3"/>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A16" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16" s="14"/>
-      <c r="J16" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="K16" s="17" t="s">
-        <v>195</v>
-      </c>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="11"/>
-      <c r="O16" s="11"/>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="11"/>
-      <c r="R16" s="11"/>
-      <c r="S16" s="21" t="s">
-        <v>227</v>
-      </c>
-      <c r="T16" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="U16" s="14" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A17" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>177</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" s="14"/>
-      <c r="J17" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="K17" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="11"/>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="11"/>
-      <c r="R17" s="11"/>
-      <c r="S17" s="21"/>
-      <c r="T17" s="19"/>
-      <c r="U17" s="14"/>
+      <c r="K17" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="15"/>
+      <c r="T17" s="21"/>
+      <c r="U17" s="19"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="J18" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="K18" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="S18" s="21" t="s">
-        <v>226</v>
-      </c>
-      <c r="T18" s="19"/>
-      <c r="U18" s="14"/>
+        <v>176</v>
+      </c>
+      <c r="K18" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="S18" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="T18" s="21"/>
+      <c r="U18" s="19"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="15" t="s">
-        <v>96</v>
+      <c r="B19" s="11" t="s">
+        <v>93</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>8</v>
@@ -1999,23 +2056,23 @@
         <v>19</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="K19" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="S19" s="21" t="s">
-        <v>190</v>
-      </c>
-      <c r="T19" s="19"/>
-      <c r="U19" s="14"/>
+        <v>177</v>
+      </c>
+      <c r="K19" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="S19" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="T19" s="21"/>
+      <c r="U19" s="19"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="15" t="s">
-        <v>97</v>
+      <c r="B20" s="11" t="s">
+        <v>94</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>8</v>
@@ -2033,27 +2090,27 @@
         <v>19</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="K20" s="17" t="s">
-        <v>136</v>
+        <v>178</v>
+      </c>
+      <c r="K20" s="13" t="s">
+        <v>133</v>
       </c>
       <c r="S20" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="T20" s="22" t="s">
+        <v>216</v>
+      </c>
+      <c r="U20" s="19" t="s">
         <v>223</v>
       </c>
-      <c r="T20" s="20" t="s">
-        <v>222</v>
-      </c>
-      <c r="U20" s="14" t="s">
-        <v>229</v>
-      </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="15" t="s">
-        <v>98</v>
+      <c r="B21" s="11" t="s">
+        <v>95</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>8</v>
@@ -2071,23 +2128,23 @@
         <v>19</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="K21" s="17" t="s">
-        <v>197</v>
+        <v>179</v>
+      </c>
+      <c r="K21" s="13" t="s">
+        <v>191</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="T21" s="20"/>
-      <c r="U21" s="14"/>
+        <v>218</v>
+      </c>
+      <c r="T21" s="22"/>
+      <c r="U21" s="19"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="15" t="s">
-        <v>99</v>
+      <c r="B22" s="11" t="s">
+        <v>96</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>8</v>
@@ -2105,21 +2162,21 @@
         <v>19</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="K22" s="17" t="s">
-        <v>198</v>
+        <v>180</v>
+      </c>
+      <c r="K22" s="13" t="s">
+        <v>192</v>
       </c>
       <c r="S22" s="2"/>
-      <c r="T22" s="20"/>
-      <c r="U22" s="14"/>
+      <c r="T22" s="22"/>
+      <c r="U22" s="19"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B23" s="15" t="s">
-        <v>100</v>
+      <c r="B23" s="11" t="s">
+        <v>97</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>8</v>
@@ -2137,21 +2194,21 @@
         <v>11</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="K23" s="17" t="s">
-        <v>199</v>
+        <v>181</v>
+      </c>
+      <c r="K23" s="13" t="s">
+        <v>193</v>
       </c>
       <c r="S23" s="2"/>
-      <c r="T23" s="20"/>
-      <c r="U23" s="14"/>
+      <c r="T23" s="22"/>
+      <c r="U23" s="19"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="15" t="s">
-        <v>101</v>
+      <c r="B24" s="11" t="s">
+        <v>98</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>8</v>
@@ -2169,21 +2226,21 @@
         <v>19</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="K24" s="17" t="s">
-        <v>200</v>
+        <v>182</v>
+      </c>
+      <c r="K24" s="13" t="s">
+        <v>194</v>
       </c>
       <c r="S24" s="2"/>
-      <c r="T24" s="20"/>
-      <c r="U24" s="14"/>
+      <c r="T24" s="22"/>
+      <c r="U24" s="19"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="15" t="s">
-        <v>102</v>
+      <c r="B25" s="11" t="s">
+        <v>99</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>8</v>
@@ -2201,21 +2258,21 @@
         <v>19</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="K25" s="17" t="s">
-        <v>201</v>
+        <v>183</v>
+      </c>
+      <c r="K25" s="13" t="s">
+        <v>195</v>
       </c>
       <c r="S25" s="2"/>
-      <c r="T25" s="20"/>
-      <c r="U25" s="14"/>
+      <c r="T25" s="22"/>
+      <c r="U25" s="19"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="15" t="s">
-        <v>103</v>
+      <c r="B26" s="11" t="s">
+        <v>100</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>8</v>
@@ -2233,23 +2290,23 @@
         <v>19</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="K26" s="17" t="s">
-        <v>202</v>
+        <v>173</v>
+      </c>
+      <c r="K26" s="13" t="s">
+        <v>196</v>
       </c>
       <c r="S26" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="T26" s="20"/>
-      <c r="U26" s="14"/>
+        <v>219</v>
+      </c>
+      <c r="T26" s="22"/>
+      <c r="U26" s="19"/>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="15" t="s">
-        <v>104</v>
+      <c r="B27" s="11" t="s">
+        <v>101</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>8</v>
@@ -2267,18 +2324,18 @@
         <v>19</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="K27" s="17" t="s">
-        <v>203</v>
+        <v>184</v>
+      </c>
+      <c r="K27" s="13" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="15" t="s">
-        <v>105</v>
+      <c r="B28" s="11" t="s">
+        <v>102</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>8</v>
@@ -2296,18 +2353,18 @@
         <v>19</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="K28" s="17" t="s">
-        <v>204</v>
+        <v>185</v>
+      </c>
+      <c r="K28" s="13" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="15" t="s">
-        <v>106</v>
+      <c r="B29" s="11" t="s">
+        <v>103</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>8</v>
@@ -2325,18 +2382,18 @@
         <v>19</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="K29" s="17" t="s">
-        <v>205</v>
+        <v>186</v>
+      </c>
+      <c r="K29" s="13" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="15" t="s">
-        <v>107</v>
+      <c r="B30" s="11" t="s">
+        <v>104</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>8</v>
@@ -2354,18 +2411,18 @@
         <v>19</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="K30" s="17" t="s">
-        <v>206</v>
+        <v>187</v>
+      </c>
+      <c r="K30" s="13" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="15" t="s">
-        <v>108</v>
+      <c r="B31" s="11" t="s">
+        <v>105</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>8</v>
@@ -2383,18 +2440,18 @@
         <v>19</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="K31" s="17" t="s">
-        <v>207</v>
+        <v>188</v>
+      </c>
+      <c r="K31" s="13" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B32" s="15" t="s">
-        <v>109</v>
+      <c r="B32" s="11" t="s">
+        <v>106</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>8</v>
@@ -2416,8 +2473,8 @@
       <c r="A33" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B33" s="15" t="s">
-        <v>110</v>
+      <c r="B33" s="11" t="s">
+        <v>107</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>8</v>
@@ -2437,10 +2494,10 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>149</v>
+        <v>145</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>146</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>8</v>
@@ -2459,11 +2516,11 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="18" t="s">
+      <c r="A36" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B36" s="15" t="s">
-        <v>111</v>
+      <c r="B36" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>8</v>
@@ -2482,11 +2539,11 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="18" t="s">
+      <c r="A37" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="B37" s="15" t="s">
-        <v>112</v>
+      <c r="B37" s="11" t="s">
+        <v>109</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>8</v>
@@ -2505,11 +2562,11 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="18" t="s">
+      <c r="A38" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="B38" s="15" t="s">
-        <v>113</v>
+      <c r="B38" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>8</v>
@@ -2528,11 +2585,11 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="18" t="s">
+      <c r="A39" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="B39" s="15" t="s">
-        <v>114</v>
+      <c r="B39" s="11" t="s">
+        <v>111</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>8</v>
@@ -2551,11 +2608,11 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="B40" s="15" t="s">
-        <v>212</v>
+      <c r="A40" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>206</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>8</v>
@@ -2574,11 +2631,11 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="B41" s="15" t="s">
-        <v>213</v>
+      <c r="A41" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>207</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>8</v>
@@ -2597,11 +2654,11 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="B42" s="15" t="s">
-        <v>214</v>
+      <c r="A42" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>208</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>8</v>
@@ -2620,11 +2677,11 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="11" t="s">
-        <v>211</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>215</v>
+      <c r="A43" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>209</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>8</v>
@@ -2643,14 +2700,14 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="18" t="s">
-        <v>234</v>
-      </c>
-      <c r="B45" s="15" t="s">
-        <v>230</v>
+      <c r="A45" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>112</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>7</v>
@@ -2659,21 +2716,21 @@
         <v>8</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="18" t="s">
-        <v>235</v>
-      </c>
-      <c r="B46" s="15" t="s">
-        <v>231</v>
+      <c r="A46" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>113</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>7</v>
@@ -2682,21 +2739,21 @@
         <v>8</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="18" t="s">
-        <v>236</v>
-      </c>
-      <c r="B47" s="15" t="s">
-        <v>232</v>
+      <c r="A47" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>114</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>7</v>
@@ -2705,21 +2762,21 @@
         <v>8</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="B48" s="15" t="s">
-        <v>233</v>
+      <c r="A48" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>7</v>
@@ -2728,18 +2785,18 @@
         <v>8</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B49" s="15" t="s">
-        <v>115</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>116</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>7</v>
@@ -2757,15 +2814,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B50" s="15" t="s">
-        <v>116</v>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>224</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>7</v>
@@ -2774,350 +2831,366 @@
         <v>8</v>
       </c>
       <c r="F50" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="B53" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="B54" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="B55" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="B56" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="B57" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="B58" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="B60" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="B61" s="26" t="s">
+        <v>260</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G63" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G50" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B51" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B52" s="15" t="s">
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B64" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G52" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B53" s="15" t="s">
+      <c r="C64" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B65" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B55" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B56" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F56" s="2" t="s">
+      <c r="C65" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F65" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G56" s="2" t="s">
+      <c r="G65" s="2" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="B57" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G57" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B58" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B59" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G59" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H59" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="18" t="s">
-        <v>217</v>
-      </c>
-      <c r="B60" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G60" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B62" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G62" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B63" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G63" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B64" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G64" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B65" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H65" s="14" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B66" s="15" t="s">
-        <v>129</v>
+        <v>87</v>
+      </c>
+      <c r="B66" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H66" s="14"/>
+        <v>42</v>
+      </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A67" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B67" s="15" t="s">
-        <v>130</v>
+      <c r="A67" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B67" s="11" t="s">
+        <v>121</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>7</v>
@@ -3126,137 +3199,139 @@
         <v>8</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H67" s="14"/>
+        <v>42</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A68" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B68" s="15" t="s">
-        <v>131</v>
+      <c r="A68" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="B68" s="11" t="s">
+        <v>212</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H68" s="16" t="s">
-        <v>94</v>
+        <v>11</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A70" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="B70" s="15" t="s">
-        <v>132</v>
+      <c r="A70" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B70" s="11" t="s">
+        <v>122</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B71" s="15" t="s">
-        <v>133</v>
+        <v>70</v>
+      </c>
+      <c r="B71" s="11" t="s">
+        <v>123</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B72" s="15" t="s">
-        <v>134</v>
+        <v>71</v>
+      </c>
+      <c r="B72" s="11" t="s">
+        <v>124</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="G72" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="B73" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F73" s="2" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B73" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="G73" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="H73" s="19" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B74" s="15" t="s">
-        <v>137</v>
+      <c r="A74" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="B74" s="11" t="s">
+        <v>126</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>7</v>
@@ -3265,21 +3340,22 @@
         <v>7</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G74" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="H74" s="19"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B75" s="15" t="s">
-        <v>138</v>
+      <c r="A75" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="B75" s="11" t="s">
+        <v>127</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>7</v>
@@ -3288,21 +3364,22 @@
         <v>7</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G75" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="H75" s="19"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B76" s="15" t="s">
-        <v>139</v>
+      <c r="A76" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="B76" s="11" t="s">
+        <v>128</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>7</v>
@@ -3311,44 +3388,24 @@
         <v>7</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G76" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A77" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B77" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G77" s="2" t="s">
-        <v>42</v>
+      <c r="H76" s="12" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A78" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B78" s="15" t="s">
-        <v>141</v>
+      <c r="A78" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B78" s="11" t="s">
+        <v>129</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>7</v>
@@ -3367,11 +3424,11 @@
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A79" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B79" s="15" t="s">
-        <v>142</v>
+      <c r="A79" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B79" s="11" t="s">
+        <v>130</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>7</v>
@@ -3390,11 +3447,11 @@
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A80" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B80" s="15" t="s">
-        <v>143</v>
+      <c r="A80" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B80" s="11" t="s">
+        <v>131</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>7</v>
@@ -3413,11 +3470,11 @@
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A81" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B81" s="15" t="s">
-        <v>144</v>
+      <c r="A81" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B81" s="11" t="s">
+        <v>132</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>7</v>
@@ -3436,11 +3493,11 @@
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A82" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B82" s="15" t="s">
-        <v>145</v>
+      <c r="A82" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B82" s="11" t="s">
+        <v>134</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>7</v>
@@ -3459,11 +3516,11 @@
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A83" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B83" s="15" t="s">
-        <v>146</v>
+      <c r="A83" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B83" s="11" t="s">
+        <v>135</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>7</v>
@@ -3482,11 +3539,11 @@
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A84" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B84" s="15" t="s">
-        <v>147</v>
+      <c r="A84" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B84" s="11" t="s">
+        <v>136</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>7</v>
@@ -3504,34 +3561,218 @@
         <v>42</v>
       </c>
     </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A85" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B85" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A86" s="2" t="s">
+      <c r="A86" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B86" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A87" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B87" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A88" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B88" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A89" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="B89" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G89" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A90" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B90" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A91" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B91" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A92" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B92" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A94" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A95" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A96" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A87" s="2" t="s">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A88" s="2" t="s">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" s="2" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A89" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A90" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A91" s="2" t="s">
-        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -3543,7 +3784,7 @@
     <mergeCell ref="Q9:R9"/>
     <mergeCell ref="S9:T9"/>
     <mergeCell ref="U9:X9"/>
-    <mergeCell ref="H65:H67"/>
+    <mergeCell ref="H73:H75"/>
     <mergeCell ref="J15:K15"/>
     <mergeCell ref="H2:H5"/>
     <mergeCell ref="H10:H13"/>

</xml_diff>

<commit_message>
Phase One Progress (4)
- Created a new virtual machine from scratch in C to run on x86-64 machines
- Changed the system call ids to match the linux system call ids instead on simply being arbitrary values
- Added system calls for opening and closing files
- Added a lea (Load Effective Address) instruction
- Bug fixes
</commit_message>
<xml_diff>
--- a/docs/ISA.xlsx
+++ b/docs/ISA.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3160" yWindow="1020" windowWidth="22600" windowHeight="15320" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1260" yWindow="700" windowWidth="22600" windowHeight="15320" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Old" sheetId="1" r:id="rId1"/>
     <sheet name="New" sheetId="2" r:id="rId2"/>
+    <sheet name="system calls" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1063" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1140" uniqueCount="365">
   <si>
     <t>Instruction</t>
   </si>
@@ -1006,13 +1007,130 @@
   </si>
   <si>
     <t>s/d</t>
+  </si>
+  <si>
+    <t>Modifier Encoding</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>word</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>quad</t>
+  </si>
+  <si>
+    <t>single float</t>
+  </si>
+  <si>
+    <t>double float</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>exit</t>
+  </si>
+  <si>
+    <t>exit_code: int</t>
+  </si>
+  <si>
+    <t>read</t>
+  </si>
+  <si>
+    <t>write</t>
+  </si>
+  <si>
+    <t>fd: uint32</t>
+  </si>
+  <si>
+    <t>count: uint64</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>close</t>
+  </si>
+  <si>
+    <t>flag: int</t>
+  </si>
+  <si>
+    <t>mode: int</t>
+  </si>
+  <si>
+    <t>malloc</t>
+  </si>
+  <si>
+    <t>0x8000</t>
+  </si>
+  <si>
+    <t>free</t>
+  </si>
+  <si>
+    <t>0x8001</t>
+  </si>
+  <si>
+    <t>ptr: raw_ptr</t>
+  </si>
+  <si>
+    <t>buf: ptr&lt;char&gt;</t>
+  </si>
+  <si>
+    <t>buf:ptr&lt;char&gt;</t>
+  </si>
+  <si>
+    <t>name: ptr&lt;char&gt;</t>
+  </si>
+  <si>
+    <t>dbg_vpu_dec</t>
+  </si>
+  <si>
+    <t>0xc000</t>
+  </si>
+  <si>
+    <t>dbg_vpu_hex</t>
+  </si>
+  <si>
+    <t>0xc001</t>
+  </si>
+  <si>
+    <t>dbg_stack</t>
+  </si>
+  <si>
+    <t>0xc002</t>
+  </si>
+  <si>
+    <t>Returns in rx</t>
+  </si>
+  <si>
+    <t>raw_ptr</t>
+  </si>
+  <si>
+    <t>int32</t>
+  </si>
+  <si>
+    <t>fd: int32</t>
+  </si>
+  <si>
+    <t>call*</t>
+  </si>
+  <si>
+    <t>indirect call (from register)</t>
+  </si>
+  <si>
+    <t>lea</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1029,6 +1147,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Monaco"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Monaco"/>
@@ -1144,7 +1268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1198,6 +1322,34 @@
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1228,22 +1380,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1571,21 +1711,21 @@
       <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="M1" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20"/>
-      <c r="X1" s="20"/>
-      <c r="Y1" s="20"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
+      <c r="Y1" s="30"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
@@ -1612,7 +1752,7 @@
       <c r="H2" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="I2" s="35" t="s">
         <v>213</v>
       </c>
       <c r="K2" s="1" t="s">
@@ -1624,18 +1764,18 @@
       <c r="M2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="N2" s="20" t="s">
+      <c r="N2" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20" t="s">
+      <c r="O2" s="30"/>
+      <c r="P2" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20" t="s">
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="S2" s="20"/>
+      <c r="S2" s="30"/>
       <c r="T2" s="1" t="s">
         <v>54</v>
       </c>
@@ -1677,7 +1817,7 @@
       <c r="H3" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="I3" s="25"/>
+      <c r="I3" s="35"/>
       <c r="K3" s="7" t="s">
         <v>20</v>
       </c>
@@ -1693,18 +1833,18 @@
       <c r="O3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="P3" s="22" t="s">
+      <c r="P3" s="32" t="s">
         <v>210</v>
       </c>
-      <c r="Q3" s="22"/>
-      <c r="R3" s="22"/>
-      <c r="S3" s="22"/>
-      <c r="T3" s="22"/>
-      <c r="U3" s="22"/>
-      <c r="V3" s="22"/>
-      <c r="W3" s="22"/>
-      <c r="X3" s="22"/>
-      <c r="Y3" s="22"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="32"/>
+      <c r="S3" s="32"/>
+      <c r="T3" s="32"/>
+      <c r="U3" s="32"/>
+      <c r="V3" s="32"/>
+      <c r="W3" s="32"/>
+      <c r="X3" s="32"/>
+      <c r="Y3" s="32"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
@@ -1728,7 +1868,7 @@
       <c r="H4" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="I4" s="25"/>
+      <c r="I4" s="35"/>
       <c r="K4" s="2" t="s">
         <v>43</v>
       </c>
@@ -1738,19 +1878,19 @@
       <c r="M4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="N4" s="22" t="s">
+      <c r="N4" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="22"/>
-      <c r="S4" s="22"/>
-      <c r="T4" s="22"/>
-      <c r="U4" s="22"/>
-      <c r="V4" s="22"/>
-      <c r="W4" s="22"/>
-      <c r="X4" s="22"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="32"/>
+      <c r="S4" s="32"/>
+      <c r="T4" s="32"/>
+      <c r="U4" s="32"/>
+      <c r="V4" s="32"/>
+      <c r="W4" s="32"/>
+      <c r="X4" s="32"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
@@ -1774,7 +1914,7 @@
       <c r="H5" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="I5" s="25"/>
+      <c r="I5" s="35"/>
       <c r="K5" s="7" t="s">
         <v>19</v>
       </c>
@@ -1949,24 +2089,24 @@
       <c r="O9" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="P9" s="21" t="s">
+      <c r="P9" s="31" t="s">
         <v>261</v>
       </c>
-      <c r="Q9" s="21"/>
-      <c r="R9" s="22" t="s">
+      <c r="Q9" s="31"/>
+      <c r="R9" s="32" t="s">
         <v>233</v>
       </c>
-      <c r="S9" s="22"/>
-      <c r="T9" s="23" t="s">
+      <c r="S9" s="32"/>
+      <c r="T9" s="33" t="s">
         <v>234</v>
       </c>
-      <c r="U9" s="23"/>
-      <c r="V9" s="24" t="s">
+      <c r="U9" s="33"/>
+      <c r="V9" s="34" t="s">
         <v>235</v>
       </c>
-      <c r="W9" s="24"/>
-      <c r="X9" s="24"/>
-      <c r="Y9" s="24"/>
+      <c r="W9" s="34"/>
+      <c r="X9" s="34"/>
+      <c r="Y9" s="34"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
@@ -1990,7 +2130,7 @@
       <c r="H10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I10" s="25" t="s">
+      <c r="I10" s="35" t="s">
         <v>236</v>
       </c>
       <c r="K10" s="7"/>
@@ -2025,7 +2165,7 @@
       <c r="H11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="25"/>
+      <c r="I11" s="35"/>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="9"/>
@@ -2058,7 +2198,7 @@
       <c r="H12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I12" s="25"/>
+      <c r="I12" s="35"/>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
       <c r="M12" s="9"/>
@@ -2091,7 +2231,7 @@
       <c r="H13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I13" s="25"/>
+      <c r="I13" s="35"/>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
       <c r="M13" s="9"/>
@@ -2124,7 +2264,7 @@
       <c r="H14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I14" s="19" t="s">
+      <c r="I14" s="29" t="s">
         <v>236</v>
       </c>
       <c r="K14" s="7"/>
@@ -2159,11 +2299,11 @@
       <c r="H15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I15" s="19"/>
-      <c r="K15" s="20" t="s">
+      <c r="I15" s="29"/>
+      <c r="K15" s="30" t="s">
         <v>172</v>
       </c>
-      <c r="L15" s="20"/>
+      <c r="L15" s="30"/>
       <c r="M15" s="9"/>
       <c r="N15" s="9"/>
       <c r="O15" s="9"/>
@@ -2171,11 +2311,11 @@
       <c r="Q15" s="9"/>
       <c r="R15" s="9"/>
       <c r="S15" s="9"/>
-      <c r="T15" s="20" t="s">
+      <c r="T15" s="30" t="s">
         <v>214</v>
       </c>
-      <c r="U15" s="20"/>
-      <c r="V15" s="20"/>
+      <c r="U15" s="30"/>
+      <c r="V15" s="30"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
@@ -2199,7 +2339,7 @@
       <c r="H16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I16" s="19"/>
+      <c r="I16" s="29"/>
       <c r="K16" s="7" t="s">
         <v>174</v>
       </c>
@@ -2216,10 +2356,10 @@
       <c r="T16" s="15" t="s">
         <v>221</v>
       </c>
-      <c r="U16" s="26" t="s">
+      <c r="U16" s="36" t="s">
         <v>215</v>
       </c>
-      <c r="V16" s="19" t="s">
+      <c r="V16" s="29" t="s">
         <v>222</v>
       </c>
     </row>
@@ -2245,7 +2385,7 @@
       <c r="H17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I17" s="19"/>
+      <c r="I17" s="29"/>
       <c r="K17" s="7" t="s">
         <v>175</v>
       </c>
@@ -2260,8 +2400,8 @@
       <c r="R17" s="9"/>
       <c r="S17" s="9"/>
       <c r="T17" s="15"/>
-      <c r="U17" s="26"/>
-      <c r="V17" s="19"/>
+      <c r="U17" s="36"/>
+      <c r="V17" s="29"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="K18" s="2" t="s">
@@ -2273,8 +2413,8 @@
       <c r="T18" s="15" t="s">
         <v>220</v>
       </c>
-      <c r="U18" s="26"/>
-      <c r="V18" s="19"/>
+      <c r="U18" s="36"/>
+      <c r="V18" s="29"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
@@ -2307,8 +2447,8 @@
       <c r="T19" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="U19" s="26"/>
-      <c r="V19" s="19"/>
+      <c r="U19" s="36"/>
+      <c r="V19" s="29"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
@@ -2341,10 +2481,10 @@
       <c r="T20" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="U20" s="27" t="s">
+      <c r="U20" s="37" t="s">
         <v>216</v>
       </c>
-      <c r="V20" s="19" t="s">
+      <c r="V20" s="29" t="s">
         <v>223</v>
       </c>
     </row>
@@ -2379,8 +2519,8 @@
       <c r="T21" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="U21" s="27"/>
-      <c r="V21" s="19"/>
+      <c r="U21" s="37"/>
+      <c r="V21" s="29"/>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
@@ -2411,8 +2551,8 @@
         <v>192</v>
       </c>
       <c r="T22" s="2"/>
-      <c r="U22" s="27"/>
-      <c r="V22" s="19"/>
+      <c r="U22" s="37"/>
+      <c r="V22" s="29"/>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
@@ -2443,8 +2583,8 @@
         <v>193</v>
       </c>
       <c r="T23" s="2"/>
-      <c r="U23" s="27"/>
-      <c r="V23" s="19"/>
+      <c r="U23" s="37"/>
+      <c r="V23" s="29"/>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
@@ -2475,8 +2615,8 @@
         <v>194</v>
       </c>
       <c r="T24" s="2"/>
-      <c r="U24" s="27"/>
-      <c r="V24" s="19"/>
+      <c r="U24" s="37"/>
+      <c r="V24" s="29"/>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
@@ -2507,8 +2647,8 @@
         <v>195</v>
       </c>
       <c r="T25" s="2"/>
-      <c r="U25" s="27"/>
-      <c r="V25" s="19"/>
+      <c r="U25" s="37"/>
+      <c r="V25" s="29"/>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
@@ -2541,8 +2681,8 @@
       <c r="T26" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="U26" s="27"/>
-      <c r="V26" s="19"/>
+      <c r="U26" s="37"/>
+      <c r="V26" s="29"/>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
@@ -3565,7 +3705,7 @@
       <c r="H73" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I73" s="19" t="s">
+      <c r="I73" s="29" t="s">
         <v>89</v>
       </c>
     </row>
@@ -3591,7 +3731,7 @@
       <c r="H74" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I74" s="19"/>
+      <c r="I74" s="29"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="14" t="s">
@@ -3615,7 +3755,7 @@
       <c r="H75" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I75" s="19"/>
+      <c r="I75" s="29"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="14" t="s">
@@ -4047,10 +4187,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X55"/>
+  <dimension ref="A1:Y57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4060,16 +4200,17 @@
     <col min="3" max="3" width="10.83203125" style="2"/>
     <col min="4" max="4" width="12" style="2" customWidth="1"/>
     <col min="5" max="5" width="14.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="5.83203125" customWidth="1"/>
-    <col min="9" max="9" width="28.6640625" customWidth="1"/>
-    <col min="10" max="10" width="5.83203125" customWidth="1"/>
-    <col min="11" max="11" width="10.83203125" style="17"/>
-    <col min="12" max="12" width="10.83203125" style="2"/>
-    <col min="13" max="16" width="5.83203125" style="2" customWidth="1"/>
-    <col min="17" max="18" width="10.83203125" style="2"/>
+    <col min="6" max="6" width="23.1640625" style="23" customWidth="1"/>
+    <col min="7" max="7" width="5.83203125" customWidth="1"/>
+    <col min="10" max="10" width="28.6640625" customWidth="1"/>
+    <col min="11" max="11" width="5.83203125" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" style="17"/>
+    <col min="13" max="13" width="10.83203125" style="2"/>
+    <col min="14" max="17" width="5.83203125" style="2" customWidth="1"/>
+    <col min="18" max="19" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -4085,48 +4226,51 @@
       <c r="E1" s="17" t="s">
         <v>266</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="F1" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="30" t="s">
         <v>172</v>
       </c>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="L1" s="2" t="s">
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="M1" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="M1" s="31" t="s">
+      <c r="N1" s="39" t="s">
         <v>286</v>
       </c>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31" t="s">
+      <c r="O1" s="39"/>
+      <c r="P1" s="39" t="s">
         <v>287</v>
       </c>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="39"/>
+      <c r="R1" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>267</v>
       </c>
@@ -4142,35 +4286,35 @@
       <c r="E2" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="I2" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="J2" s="13" t="s">
         <v>308</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="L2" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="O2" s="29" t="s">
+      <c r="P2" s="21" t="s">
         <v>280</v>
       </c>
-      <c r="P2" s="30" t="s">
+      <c r="Q2" s="22" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>314</v>
       </c>
@@ -4186,43 +4330,43 @@
       <c r="E3" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="I3" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="J3" s="13" t="s">
         <v>308</v>
       </c>
-      <c r="K3" s="17" t="s">
+      <c r="L3" s="17" t="s">
         <v>283</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="N3" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="O3" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="O3" s="8"/>
-      <c r="P3" s="30" t="s">
+      <c r="P3" s="8"/>
+      <c r="Q3" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="Q3" s="32" t="s">
+      <c r="R3" s="40" t="s">
         <v>313</v>
       </c>
-      <c r="R3" s="32"/>
-      <c r="S3" s="32"/>
-      <c r="T3" s="32"/>
-      <c r="U3" s="32"/>
-      <c r="V3" s="32"/>
-      <c r="W3" s="32"/>
-      <c r="X3" s="32"/>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="S3" s="40"/>
+      <c r="T3" s="40"/>
+      <c r="U3" s="40"/>
+      <c r="V3" s="40"/>
+      <c r="W3" s="40"/>
+      <c r="X3" s="40"/>
+      <c r="Y3" s="40"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>268</v>
       </c>
@@ -4238,40 +4382,40 @@
       <c r="E4" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="I4" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="J4" s="13" t="s">
         <v>308</v>
       </c>
-      <c r="K4" s="17" t="s">
+      <c r="L4" s="17" t="s">
         <v>284</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="N4" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="O4" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="O4" s="32" t="s">
+      <c r="P4" s="40" t="s">
         <v>313</v>
       </c>
-      <c r="P4" s="32"/>
-      <c r="Q4" s="32"/>
-      <c r="R4" s="32"/>
-      <c r="S4" s="32"/>
-      <c r="T4" s="32"/>
-      <c r="U4" s="32"/>
-      <c r="V4" s="32"/>
-      <c r="W4" s="32"/>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Q4" s="40"/>
+      <c r="R4" s="40"/>
+      <c r="S4" s="40"/>
+      <c r="T4" s="40"/>
+      <c r="U4" s="40"/>
+      <c r="V4" s="40"/>
+      <c r="W4" s="40"/>
+      <c r="X4" s="40"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>315</v>
       </c>
@@ -4287,34 +4431,35 @@
       <c r="E5" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="I5" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="J5" s="13" t="s">
         <v>308</v>
       </c>
-      <c r="K5" s="17" t="s">
+      <c r="L5" s="17" t="s">
         <v>288</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M5" s="32" t="s">
+      <c r="N5" s="40" t="s">
         <v>288</v>
       </c>
-      <c r="N5" s="32"/>
-      <c r="O5" s="32"/>
-      <c r="P5" s="32"/>
-      <c r="Q5" s="32"/>
-      <c r="R5" s="32"/>
-      <c r="S5" s="32"/>
-      <c r="T5" s="32"/>
-      <c r="U5" s="32"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="O5" s="40"/>
+      <c r="P5" s="40"/>
+      <c r="Q5" s="40"/>
+      <c r="R5" s="40"/>
+      <c r="S5" s="40"/>
+      <c r="T5" s="40"/>
+      <c r="U5" s="40"/>
+      <c r="V5" s="40"/>
+      <c r="W5" s="40"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>269</v>
       </c>
@@ -4330,23 +4475,23 @@
       <c r="E6" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="I6" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="J6" s="13" t="s">
         <v>308</v>
       </c>
-      <c r="K6" s="17" t="s">
+      <c r="L6" s="17" t="s">
         <v>300</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>299</v>
       </c>
@@ -4362,28 +4507,28 @@
       <c r="E7" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="I7" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="J7" s="13" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="G8" s="2" t="s">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="H8" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="I8" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="J8" s="13" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>1</v>
       </c>
@@ -4399,17 +4544,17 @@
       <c r="E9" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="I9" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="J9" s="13" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>21</v>
       </c>
@@ -4425,17 +4570,17 @@
       <c r="E10" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="H10" s="13" t="s">
+      <c r="I10" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="J10" s="13" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>24</v>
       </c>
@@ -4451,17 +4596,17 @@
       <c r="E11" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="I11" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="J11" s="13" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>25</v>
       </c>
@@ -4477,17 +4622,21 @@
       <c r="E12" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="I12" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="J12" s="13" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="T12" s="30" t="s">
+        <v>326</v>
+      </c>
+      <c r="U12" s="30"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
         <v>64</v>
       </c>
@@ -4498,33 +4647,39 @@
         <v>206</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="I13" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="I13" s="13" t="s">
+      <c r="J13" s="13" t="s">
         <v>317</v>
       </c>
-      <c r="K13" s="17" t="s">
+      <c r="L13" s="17" t="s">
         <v>300</v>
       </c>
-      <c r="L13" s="33" t="s">
+      <c r="M13" s="38" t="s">
         <v>302</v>
       </c>
-      <c r="M13" s="33"/>
-      <c r="N13" s="33"/>
-      <c r="O13" s="33"/>
-      <c r="P13" s="33"/>
-      <c r="Q13" s="33"/>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="N13" s="38"/>
+      <c r="O13" s="38"/>
+      <c r="P13" s="38"/>
+      <c r="Q13" s="38"/>
+      <c r="R13" s="38"/>
+      <c r="T13" t="s">
+        <v>327</v>
+      </c>
+      <c r="U13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>67</v>
       </c>
@@ -4540,28 +4695,34 @@
       <c r="E14" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="I14" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="J14" s="13" t="s">
         <v>309</v>
       </c>
-      <c r="K14" s="17" t="s">
+      <c r="L14" s="17" t="s">
         <v>288</v>
       </c>
-      <c r="L14" s="33" t="s">
+      <c r="M14" s="38" t="s">
         <v>301</v>
       </c>
-      <c r="M14" s="33"/>
-      <c r="N14" s="33"/>
-      <c r="O14" s="33"/>
-      <c r="P14" s="33"/>
-      <c r="Q14" s="33"/>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="N14" s="38"/>
+      <c r="O14" s="38"/>
+      <c r="P14" s="38"/>
+      <c r="Q14" s="38"/>
+      <c r="R14" s="38"/>
+      <c r="T14" t="s">
+        <v>328</v>
+      </c>
+      <c r="U14" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>68</v>
       </c>
@@ -4577,28 +4738,34 @@
       <c r="E15" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="H15" s="13" t="s">
+      <c r="I15" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="I15" s="13" t="s">
+      <c r="J15" s="13" t="s">
         <v>309</v>
       </c>
-      <c r="K15" s="17" t="s">
+      <c r="L15" s="17" t="s">
         <v>284</v>
       </c>
-      <c r="L15" s="33" t="s">
+      <c r="M15" s="38" t="s">
         <v>303</v>
       </c>
-      <c r="M15" s="33"/>
-      <c r="N15" s="33"/>
-      <c r="O15" s="33"/>
-      <c r="P15" s="33"/>
-      <c r="Q15" s="33"/>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="N15" s="38"/>
+      <c r="O15" s="38"/>
+      <c r="P15" s="38"/>
+      <c r="Q15" s="38"/>
+      <c r="R15" s="38"/>
+      <c r="T15" t="s">
+        <v>329</v>
+      </c>
+      <c r="U15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>88</v>
       </c>
@@ -4614,28 +4781,34 @@
       <c r="E16" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="H16" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="H16" s="13" t="s">
+      <c r="I16" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="I16" s="13" t="s">
+      <c r="J16" s="13" t="s">
         <v>318</v>
       </c>
-      <c r="K16" s="17" t="s">
+      <c r="L16" s="17" t="s">
         <v>283</v>
       </c>
-      <c r="L16" s="33" t="s">
+      <c r="M16" s="38" t="s">
         <v>304</v>
       </c>
-      <c r="M16" s="33"/>
-      <c r="N16" s="33"/>
-      <c r="O16" s="33"/>
-      <c r="P16" s="33"/>
-      <c r="Q16" s="33"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="N16" s="38"/>
+      <c r="O16" s="38"/>
+      <c r="P16" s="38"/>
+      <c r="Q16" s="38"/>
+      <c r="R16" s="38"/>
+      <c r="T16" t="s">
+        <v>330</v>
+      </c>
+      <c r="U16" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
         <v>60</v>
       </c>
@@ -4651,28 +4824,34 @@
       <c r="E17" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="H17" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="H17" s="13" t="s">
+      <c r="I17" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="I17" s="13" t="s">
+      <c r="J17" s="13" t="s">
         <v>319</v>
       </c>
-      <c r="K17" s="17" t="s">
+      <c r="L17" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="L17" s="33" t="s">
+      <c r="M17" s="38" t="s">
         <v>305</v>
       </c>
-      <c r="M17" s="33"/>
-      <c r="N17" s="33"/>
-      <c r="O17" s="33"/>
-      <c r="P17" s="33"/>
-      <c r="Q17" s="33"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="N17" s="38"/>
+      <c r="O17" s="38"/>
+      <c r="P17" s="38"/>
+      <c r="Q17" s="38"/>
+      <c r="R17" s="38"/>
+      <c r="T17" t="s">
+        <v>331</v>
+      </c>
+      <c r="U17" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>61</v>
       </c>
@@ -4688,19 +4867,25 @@
       <c r="E18" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="K18" s="17" t="s">
+      <c r="L18" s="17" t="s">
         <v>306</v>
       </c>
-      <c r="L18" s="33" t="s">
+      <c r="M18" s="38" t="s">
         <v>311</v>
       </c>
-      <c r="M18" s="33"/>
-      <c r="N18" s="33"/>
-      <c r="O18" s="33"/>
-      <c r="P18" s="33"/>
-      <c r="Q18" s="33"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="N18" s="38"/>
+      <c r="O18" s="38"/>
+      <c r="P18" s="38"/>
+      <c r="Q18" s="38"/>
+      <c r="R18" s="38"/>
+      <c r="T18" t="s">
+        <v>332</v>
+      </c>
+      <c r="U18" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
         <v>62</v>
       </c>
@@ -4716,19 +4901,19 @@
       <c r="E19" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="K19" s="17" t="s">
+      <c r="L19" s="17" t="s">
         <v>307</v>
       </c>
-      <c r="L19" s="33" t="s">
+      <c r="M19" s="38" t="s">
         <v>312</v>
       </c>
-      <c r="M19" s="33"/>
-      <c r="N19" s="33"/>
-      <c r="O19" s="33"/>
-      <c r="P19" s="33"/>
-      <c r="Q19" s="33"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="N19" s="38"/>
+      <c r="O19" s="38"/>
+      <c r="P19" s="38"/>
+      <c r="Q19" s="38"/>
+      <c r="R19" s="38"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
         <v>63</v>
       </c>
@@ -4744,15 +4929,15 @@
       <c r="E20" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="L20" s="28"/>
-      <c r="M20" s="28"/>
-      <c r="N20" s="28"/>
-      <c r="O20" s="28"/>
-      <c r="P20" s="28"/>
-      <c r="Q20" s="28"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A21" s="14" t="s">
+      <c r="M20" s="20"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="20"/>
+      <c r="P20" s="20"/>
+      <c r="Q20" s="20"/>
+      <c r="R20" s="20"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A21" s="24" t="s">
         <v>202</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -4768,8 +4953,8 @@
         <v>282</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A22" s="14" t="s">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A22" s="24" t="s">
         <v>203</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -4785,8 +4970,8 @@
         <v>282</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A23" s="34" t="s">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A23" s="24" t="s">
         <v>204</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -4802,8 +4987,8 @@
         <v>282</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A24" s="34" t="s">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A24" s="24" t="s">
         <v>205</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -4819,7 +5004,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
         <v>316</v>
       </c>
@@ -4836,7 +5021,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="16" t="s">
         <v>320</v>
       </c>
@@ -4853,7 +5038,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="16" t="s">
         <v>321</v>
       </c>
@@ -4870,7 +5055,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="s">
         <v>322</v>
       </c>
@@ -4887,7 +5072,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" s="16" t="s">
         <v>323</v>
       </c>
@@ -4904,7 +5089,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" s="16" t="s">
         <v>324</v>
       </c>
@@ -4921,7 +5106,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
         <v>48</v>
       </c>
@@ -4938,7 +5123,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33" s="14" t="s">
         <v>47</v>
       </c>
@@ -4955,7 +5140,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
         <v>49</v>
       </c>
@@ -4972,7 +5157,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35" s="14" t="s">
         <v>211</v>
       </c>
@@ -4989,7 +5174,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
         <v>153</v>
       </c>
@@ -5006,7 +5191,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="s">
         <v>69</v>
       </c>
@@ -5023,7 +5208,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A38" s="14" t="s">
         <v>45</v>
       </c>
@@ -5040,7 +5225,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39" s="14" t="s">
         <v>46</v>
       </c>
@@ -5057,49 +5242,69 @@
         <v>284</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A40" s="14" t="s">
+        <v>362</v>
+      </c>
+      <c r="B40" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="23" t="s">
+        <v>226</v>
+      </c>
+      <c r="D40" s="23" t="s">
+        <v>284</v>
+      </c>
+      <c r="E40" s="23" t="s">
+        <v>284</v>
+      </c>
+      <c r="F40" s="23" t="s">
+        <v>363</v>
+      </c>
+      <c r="L40" s="19"/>
+      <c r="M40" s="23"/>
+      <c r="N40" s="23"/>
+      <c r="O40" s="23"/>
+      <c r="P40" s="23"/>
+      <c r="Q40" s="23"/>
+      <c r="R40" s="23"/>
+      <c r="S40" s="23"/>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A41" s="14" t="s">
+        <v>364</v>
+      </c>
+      <c r="B41" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D41" s="26" t="s">
+        <v>282</v>
+      </c>
+      <c r="E41" s="26" t="s">
+        <v>282</v>
+      </c>
+      <c r="F41" s="26"/>
+      <c r="L41" s="25"/>
+      <c r="M41" s="26"/>
+      <c r="N41" s="26"/>
+      <c r="O41" s="26"/>
+      <c r="P41" s="26"/>
+      <c r="Q41" s="26"/>
+      <c r="R41" s="26"/>
+      <c r="S41" s="26"/>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A43" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" s="11" t="s">
+      <c r="B43" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="11" t="s">
         <v>129</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>131</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>288</v>
@@ -5108,15 +5313,15 @@
         <v>288</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A44" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>288</v>
@@ -5125,15 +5330,15 @@
         <v>288</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A45" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>288</v>
@@ -5142,15 +5347,15 @@
         <v>288</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A46" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>288</v>
@@ -5159,15 +5364,15 @@
         <v>288</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A47" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>288</v>
@@ -5176,15 +5381,15 @@
         <v>288</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A48" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>288</v>
@@ -5195,13 +5400,13 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>288</v>
@@ -5212,13 +5417,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>288</v>
@@ -5229,13 +5434,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>288</v>
@@ -5246,13 +5451,13 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>288</v>
@@ -5263,13 +5468,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>288</v>
@@ -5280,13 +5485,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>288</v>
@@ -5297,13 +5502,13 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>288</v>
@@ -5312,22 +5517,287 @@
         <v>288</v>
       </c>
     </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>288</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="L19:Q19"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="L13:Q13"/>
-    <mergeCell ref="L14:Q14"/>
-    <mergeCell ref="L15:Q15"/>
-    <mergeCell ref="L16:Q16"/>
-    <mergeCell ref="L17:Q17"/>
-    <mergeCell ref="L18:Q18"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="O4:W4"/>
-    <mergeCell ref="Q3:X3"/>
-    <mergeCell ref="M5:U5"/>
+  <mergeCells count="14">
+    <mergeCell ref="M19:R19"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="M13:R13"/>
+    <mergeCell ref="M14:R14"/>
+    <mergeCell ref="M15:R15"/>
+    <mergeCell ref="M16:R16"/>
+    <mergeCell ref="M17:R17"/>
+    <mergeCell ref="M18:R18"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="P4:X4"/>
+    <mergeCell ref="R3:Y3"/>
+    <mergeCell ref="T12:U12"/>
+    <mergeCell ref="N5:W5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="16.33203125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="11"/>
+    <col min="4" max="8" width="17" style="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="27" t="s">
+        <v>333</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>358</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>177</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>359</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>339</v>
+      </c>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+    </row>
+    <row r="3" spans="1:8" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>346</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>348</v>
+      </c>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+    </row>
+    <row r="4" spans="1:8" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>352</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>353</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+    </row>
+    <row r="5" spans="1:8" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>354</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>355</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+    </row>
+    <row r="6" spans="1:8" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>356</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>339</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+    </row>
+    <row r="7" spans="1:8" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>334</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>336</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>338</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>349</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>337</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>338</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>350</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>340</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>351</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>342</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>341</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>351</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>